<commit_message>
updated v2 framework code
</commit_message>
<xml_diff>
--- a/DataFiles/TestData.xlsx
+++ b/DataFiles/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11008"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B4DAC41-44D6-5742-B051-94F5CD670811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BABC9C-C2E9-2E46-97CA-E78B37C61AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,10 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>logind3</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>DataTwo</t>
   </si>
@@ -28,18 +25,9 @@
     <t>DataOne</t>
   </si>
   <si>
-    <t>DataThree</t>
-  </si>
-  <si>
     <t>TestCase</t>
   </si>
   <si>
-    <t>user1</t>
-  </si>
-  <si>
-    <t>user2</t>
-  </si>
-  <si>
     <t>TC1</t>
   </si>
   <si>
@@ -52,38 +40,71 @@
     <t>TC4</t>
   </si>
   <si>
+    <t>standard_user</t>
+  </si>
+  <si>
+    <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>locked_out_user</t>
+  </si>
+  <si>
+    <t>problem_user</t>
+  </si>
+  <si>
+    <t>performance_glitch_user</t>
+  </si>
+  <si>
+    <t>error_user</t>
+  </si>
+  <si>
+    <t>visual_user</t>
+  </si>
+  <si>
+    <t>TC5</t>
+  </si>
+  <si>
+    <t>TC6</t>
+  </si>
+  <si>
+    <t>TC7</t>
+  </si>
+  <si>
+    <t>TC8</t>
+  </si>
+  <si>
+    <t>TC9</t>
+  </si>
+  <si>
+    <t>TC10</t>
+  </si>
+  <si>
+    <t>invalid_user</t>
+  </si>
+  <si>
     <t>pass1</t>
   </si>
   <si>
-    <t>logind1</t>
-  </si>
-  <si>
     <t>pass2</t>
   </si>
   <si>
-    <t>logind2</t>
-  </si>
-  <si>
-    <t>user3</t>
-  </si>
-  <si>
-    <t>pass3</t>
-  </si>
-  <si>
-    <t>user4</t>
-  </si>
-  <si>
-    <t>pass4</t>
-  </si>
-  <si>
-    <t>logind4</t>
+    <t>valid_user</t>
+  </si>
+  <si>
+    <t>invalid_pass</t>
+  </si>
+  <si>
+    <t>new_user</t>
+  </si>
+  <si>
+    <t>new_pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +116,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,7 +141,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -137,15 +164,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,92 +489,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="B8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="B9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="B10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="B11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="hack@gmail.com" xr:uid="{220F6379-EC3C-FE44-BC94-451BE03FE47D}"/>
+    <hyperlink ref="C2" r:id="rId2" display="Hackathon@123" xr:uid="{F91BB6EB-EB19-A341-BA76-1BE3D7158B7E}"/>
+    <hyperlink ref="C3:C6" r:id="rId3" display="Hackathon@123" xr:uid="{1C884B22-739A-B745-81AF-2A20C6D3B716}"/>
+    <hyperlink ref="C7" r:id="rId4" display="Hackathon@123" xr:uid="{AD62E7A9-4E64-A340-9053-64809E90451E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updated v3 framework code
</commit_message>
<xml_diff>
--- a/DataFiles/TestData.xlsx
+++ b/DataFiles/TestData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10526"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BABC9C-C2E9-2E46-97CA-E78B37C61AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E8DF40-86A4-8741-88B7-F0EEE060F946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -141,7 +141,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -164,27 +164,15 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,7 +480,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -583,10 +571,10 @@
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -594,10 +582,10 @@
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -605,10 +593,10 @@
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -616,10 +604,10 @@
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>